<commit_message>
Update on the weight tables
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -68,13 +68,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,13 +478,10 @@
           <t>Warm-Up/Follow-Up Exercise</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="2">
+      <c r="C2" s="2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E2">
         <f>C2*D2</f>
         <v/>
       </c>
@@ -499,13 +495,10 @@
           <t>Quizzes (best 5 of 6)</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="2">
+      <c r="C3" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
         <f>C3*D3</f>
         <v/>
       </c>
@@ -519,13 +512,10 @@
           <t>In-Class Test 1</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="n"/>
-      <c r="E4" s="2">
+      <c r="C4" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
         <f>C4*D4</f>
         <v/>
       </c>
@@ -539,13 +529,10 @@
           <t>In-Class Test 2</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="n"/>
-      <c r="E5" s="2">
+      <c r="C5" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
         <f>C5*D5</f>
         <v/>
       </c>
@@ -559,14 +546,22 @@
           <t>Final Exam</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="2">
+      <c r="C6" s="2" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="E6">
         <f>C6*D6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="E7">
+        <f>E2+E3+E4+E5+E6</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Converted it to function
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Course Weight" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Course Weight" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>